<commit_message>
grado 11 - guion 08 - solicitud de imágenes
Del manuscrito. Total: 11 imágenes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/SolicitudGrafica - CS_11_01_REC250.xlsx
+++ b/fuentes/contenidos/grado11/guion01/SolicitudGrafica - CS_11_01_REC250.xlsx
@@ -1490,6 +1490,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1574,18 +1586,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -2433,9 +2433,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2473,14 +2473,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="F2" s="81" t="s">
+      <c r="D2" s="93"/>
+      <c r="F2" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="82"/>
+      <c r="G2" s="86"/>
       <c r="H2" s="54"/>
       <c r="I2" s="54"/>
       <c r="J2" s="15"/>
@@ -2490,12 +2490,12 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="90">
+      <c r="C3" s="94">
         <v>11</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="84"/>
+      <c r="D3" s="95"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="88"/>
       <c r="H3" s="54"/>
       <c r="I3" s="54"/>
       <c r="J3" s="15"/>
@@ -2505,10 +2505,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="91"/>
+      <c r="D4" s="95"/>
       <c r="E4" s="5"/>
       <c r="F4" s="53" t="s">
         <v>55</v>
@@ -2526,10 +2526,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="97" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="94"/>
+      <c r="D5" s="98"/>
       <c r="E5" s="5"/>
       <c r="F5" s="51" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2580,12 +2580,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="87"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="91"/>
       <c r="J8" s="17"/>
       <c r="K8" s="11"/>
       <c r="L8" s="2"/>
@@ -2598,7 +2598,7 @@
       <c r="A9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="113" t="s">
+      <c r="B9" s="81" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="23" t="s">
@@ -2665,7 +2665,7 @@
       <c r="J10" s="79" t="s">
         <v>150</v>
       </c>
-      <c r="K10" s="114" t="s">
+      <c r="K10" s="82" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2702,7 +2702,7 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J11" s="115" t="s">
+      <c r="J11" s="83" t="s">
         <v>153</v>
       </c>
       <c r="K11" s="14"/>
@@ -2740,10 +2740,10 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J12" s="114" t="s">
+      <c r="J12" s="82" t="s">
         <v>154</v>
       </c>
-      <c r="K12" s="114" t="s">
+      <c r="K12" s="82" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2780,10 +2780,10 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J13" s="114" t="s">
+      <c r="J13" s="82" t="s">
         <v>155</v>
       </c>
-      <c r="K13" s="114" t="s">
+      <c r="K13" s="82" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2820,7 +2820,7 @@
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J14" s="114" t="s">
+      <c r="J14" s="82" t="s">
         <v>157</v>
       </c>
       <c r="K14" s="18"/>
@@ -2858,7 +2858,7 @@
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J15" s="116" t="s">
+      <c r="J15" s="84" t="s">
         <v>158</v>
       </c>
       <c r="K15" s="20"/>
@@ -2870,7 +2870,7 @@
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="26" t="str">
-        <f t="shared" ref="C11:C22" si="3">IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C16:C22" si="3">IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D16" s="13"/>
@@ -5332,25 +5332,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="103"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="45"/>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="101"/>
-      <c r="E2" s="102"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="106"/>
       <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -5358,11 +5358,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="45"/>
-      <c r="C3" s="106" t="s">
+      <c r="C3" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="107"/>
-      <c r="E3" s="108"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="112"/>
       <c r="F3" s="46"/>
       <c r="H3" s="36" t="s">
         <v>18</v>
@@ -5413,11 +5413,11 @@
       <c r="C5" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="109" t="str">
+      <c r="D5" s="113" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="110"/>
+      <c r="E5" s="114"/>
       <c r="F5" s="46"/>
       <c r="H5" s="36" t="s">
         <v>22</v>
@@ -5462,12 +5462,12 @@
       <c r="C7" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="95" t="str">
+      <c r="D7" s="99" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="96"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="100"/>
       <c r="H7" s="36" t="s">
         <v>24</v>
       </c>
@@ -5561,14 +5561,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="98"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="99"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="103"/>
       <c r="I13" s="36" t="s">
         <v>33</v>
       </c>
@@ -5601,12 +5601,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="45"/>
-      <c r="C15" s="100" t="s">
+      <c r="C15" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="102"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="J15" s="36">
         <v>12</v>
       </c>
@@ -5646,12 +5646,12 @@
       <c r="C17" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="103" t="str">
+      <c r="D17" s="107" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="104"/>
-      <c r="F17" s="105"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="109"/>
       <c r="J17" s="36">
         <v>14</v>
       </c>
@@ -5667,12 +5667,12 @@
       <c r="C18" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="95" t="str">
+      <c r="D18" s="99" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="95"/>
-      <c r="F18" s="96"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="100"/>
       <c r="J18" s="36">
         <v>15</v>
       </c>
@@ -6064,41 +6064,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="111" t="s">
+      <c r="C1" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="111" t="s">
+      <c r="D1" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="111" t="s">
+      <c r="E1" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="111" t="s">
+      <c r="F1" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="111" t="s">
+      <c r="G1" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="112" t="s">
+      <c r="H1" s="116" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="55" t="s">
         <v>65</v>
       </c>

</xml_diff>